<commit_message>
[ADDITIONAL SCRAPING] added code to scrape more data about a player's batting performance in a match, also updated the excel sheets
</commit_message>
<xml_diff>
--- a/bin/sheets/main_db/active_players/all_formats/ActivePlayers_BAN.xlsx
+++ b/bin/sheets/main_db/active_players/all_formats/ActivePlayers_BAN.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E43"/>
+  <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -550,7 +550,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D6" t="n">
         <v>8</v>
@@ -575,7 +575,7 @@
         <v>8</v>
       </c>
       <c r="E7" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8">
@@ -590,7 +590,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
@@ -607,13 +607,13 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D9" t="n">
         <v>66</v>
       </c>
       <c r="E9" t="n">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10">
@@ -685,13 +685,13 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D13" t="n">
         <v>71</v>
       </c>
       <c r="E13" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14">
@@ -767,7 +767,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D17" t="n">
         <v>28</v>
@@ -826,7 +826,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D20" t="n">
         <v>245</v>
@@ -853,7 +853,7 @@
         <v>86</v>
       </c>
       <c r="E21" t="n">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22">
@@ -868,13 +868,13 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D22" t="n">
         <v>21</v>
       </c>
       <c r="E22" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="23">
@@ -893,7 +893,7 @@
         <v>7</v>
       </c>
       <c r="E23" t="n">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24">
@@ -954,331 +954,348 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Rony Talukdar</t>
+          <t>Rishad Hossain</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>4448</t>
+          <t>7198</t>
         </is>
       </c>
       <c r="C27" t="inlineStr"/>
       <c r="D27" t="inlineStr"/>
       <c r="E27" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Rubel Hossain</t>
+          <t>Rony Talukdar</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>3635</t>
-        </is>
-      </c>
-      <c r="C28" t="n">
-        <v>27</v>
-      </c>
-      <c r="D28" t="n">
-        <v>104</v>
-      </c>
+          <t>4448</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr"/>
+      <c r="D28" t="inlineStr"/>
       <c r="E28" t="n">
-        <v>28</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Sabbir Rahman</t>
+          <t>Rubel Hossain</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>4268</t>
+          <t>3635</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="D29" t="n">
-        <v>66</v>
+        <v>104</v>
       </c>
       <c r="E29" t="n">
-        <v>48</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Saif Hassan</t>
+          <t>Sabbir Rahman</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>5773</t>
+          <t>4268</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>6</v>
-      </c>
-      <c r="D30" t="inlineStr"/>
+        <v>11</v>
+      </c>
+      <c r="D30" t="n">
+        <v>66</v>
+      </c>
       <c r="E30" t="n">
-        <v>2</v>
+        <v>48</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Shadman Islam</t>
+          <t>Saif Hassan</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>4835</t>
+          <t>5773</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="D31" t="inlineStr"/>
-      <c r="E31" t="inlineStr"/>
+      <c r="E31" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Shakib Al Hasan</t>
+          <t>Shadman Islam</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>3426</t>
+          <t>4835</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>65</v>
-      </c>
-      <c r="D32" t="n">
-        <v>230</v>
-      </c>
-      <c r="E32" t="n">
-        <v>113</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="D32" t="inlineStr"/>
+      <c r="E32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Shamim Hossain</t>
+          <t>Shakib Al Hasan</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>6048</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr"/>
-      <c r="D33" t="inlineStr"/>
+          <t>3426</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>66</v>
+      </c>
+      <c r="D33" t="n">
+        <v>230</v>
+      </c>
       <c r="E33" t="n">
-        <v>13</v>
+        <v>115</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Shohidul Islam</t>
+          <t>Shamim Hossain</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>6455</t>
+          <t>6048</t>
         </is>
       </c>
       <c r="C34" t="inlineStr"/>
       <c r="D34" t="inlineStr"/>
       <c r="E34" t="n">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Shoriful Islam</t>
+          <t>Shohidul Islam</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>5958</t>
-        </is>
-      </c>
-      <c r="C35" t="n">
-        <v>5</v>
-      </c>
-      <c r="D35" t="n">
-        <v>14</v>
-      </c>
+          <t>6455</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr"/>
+      <c r="D35" t="inlineStr"/>
       <c r="E35" t="n">
-        <v>29</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Soumya Sarkar</t>
+          <t>Shoriful Islam</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>4362</t>
+          <t>5958</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D36" t="n">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="E36" t="n">
-        <v>72</v>
+        <v>30</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Taijul Islam</t>
+          <t>Soumya Sarkar</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>4324</t>
+          <t>4362</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="D37" t="n">
-        <v>15</v>
+        <v>61</v>
       </c>
       <c r="E37" t="n">
-        <v>2</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Tamim Iqbal</t>
+          <t>Taijul Islam</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>3461</t>
+          <t>4324</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>69</v>
+        <v>41</v>
       </c>
       <c r="D38" t="n">
-        <v>237</v>
+        <v>15</v>
       </c>
       <c r="E38" t="n">
-        <v>78</v>
+        <v>2</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Tanvir Islam</t>
+          <t>Tamim Iqbal</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>7182</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr"/>
-      <c r="D39" t="inlineStr"/>
+          <t>3461</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>70</v>
+      </c>
+      <c r="D39" t="n">
+        <v>237</v>
+      </c>
       <c r="E39" t="n">
-        <v>1</v>
+        <v>78</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Taskin Ahmed</t>
+          <t>Tanvir Islam</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>4299</t>
-        </is>
-      </c>
-      <c r="C40" t="n">
-        <v>12</v>
-      </c>
-      <c r="D40" t="n">
-        <v>57</v>
-      </c>
+          <t>7182</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr"/>
+      <c r="D40" t="inlineStr"/>
       <c r="E40" t="n">
-        <v>50</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Towhid Hridoy</t>
+          <t>Taskin Ahmed</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>7162</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr"/>
+          <t>4299</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>12</v>
+      </c>
       <c r="D41" t="n">
-        <v>3</v>
+        <v>57</v>
       </c>
       <c r="E41" t="n">
-        <v>4</v>
+        <v>52</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Yasir Ali</t>
+          <t>Towhid Hridoy</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>6456</t>
-        </is>
-      </c>
-      <c r="C42" t="n">
+          <t>7162</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr"/>
+      <c r="D42" t="n">
+        <v>3</v>
+      </c>
+      <c r="E42" t="n">
         <v>6</v>
-      </c>
-      <c r="D42" t="n">
-        <v>9</v>
-      </c>
-      <c r="E42" t="n">
-        <v>10</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
+          <t>Yasir Ali</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>6456</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>6</v>
+      </c>
+      <c r="D43" t="n">
+        <v>9</v>
+      </c>
+      <c r="E43" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
           <t>Zakir Hasan</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr">
+      <c r="B44" t="inlineStr">
         <is>
           <t>4733</t>
         </is>
       </c>
-      <c r="C43" t="n">
+      <c r="C44" t="n">
         <v>2</v>
       </c>
-      <c r="D43" t="inlineStr"/>
-      <c r="E43" t="n">
+      <c r="D44" t="inlineStr"/>
+      <c r="E44" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>